<commit_message>
Changing the way of generating the TesouroDireto links
- Applying Regex when generating the links
- Updating the excel data related to the Economic Indexers
</commit_message>
<xml_diff>
--- a/indexer_lib/data/Poupança nova mensal.xlsx
+++ b/indexer_lib/data/Poupança nova mensal.xlsx
@@ -500,7 +500,9 @@
       <c r="H2" s="3">
         <v>0.24</v>
       </c>
-      <c r="I2" s="3"/>
+      <c r="I2" s="3">
+        <v>0.3</v>
+      </c>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>

</xml_diff>

<commit_message>
Handling some exception cases in the 'Economic Indexer Widget'
- Handling some exception cases, related to the 'Initial Value' and 'Additional Interest Rate' fields, in the 'Economic Indexer Widget'
- Updating the data spreadsheets, (IPCA, SELIC, etc) with 2021 September values
</commit_message>
<xml_diff>
--- a/indexer_lib/data/Poupança nova mensal.xlsx
+++ b/indexer_lib/data/Poupança nova mensal.xlsx
@@ -423,7 +423,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -503,7 +505,9 @@
       <c r="I2" s="3">
         <v>0.3</v>
       </c>
-      <c r="J2" s="3"/>
+      <c r="J2" s="3">
+        <v>0.36</v>
+      </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>

</xml_diff>

<commit_message>
Updating the indexer lib spreadsheets with Oct/2021 data
Updating the indexer lib spreadsheets with Oct/2021 data
</commit_message>
<xml_diff>
--- a/indexer_lib/data/Poupança nova mensal.xlsx
+++ b/indexer_lib/data/Poupança nova mensal.xlsx
@@ -423,9 +423,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -508,7 +506,9 @@
       <c r="J2" s="3">
         <v>0.36</v>
       </c>
-      <c r="K2" s="3"/>
+      <c r="K2" s="3">
+        <v>0.36</v>
+      </c>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="O2" t="s">

</xml_diff>

<commit_message>
Updating all the economic indexer spreadsheet with data from Nov/2021
- Updated all the economic indexer spreadsheet with data from Nov/2021
- Removed the "Poupança antiga mensal" reference
</commit_message>
<xml_diff>
--- a/indexer_lib/data/Poupança nova mensal.xlsx
+++ b/indexer_lib/data/Poupança nova mensal.xlsx
@@ -423,7 +423,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -509,7 +511,9 @@
       <c r="K2" s="3">
         <v>0.36</v>
       </c>
-      <c r="L2" s="3"/>
+      <c r="L2" s="3">
+        <v>0.44</v>
+      </c>
       <c r="M2" s="3"/>
       <c r="O2" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Adding the IPCA and CDI values, related to the 'Renda Fixa' tab
- Added the 'getValueByPrefixedRatePlusIPCA' and 'getValueByProportionalCDI' methods
- Included an extended dataframe in the IndexerManager class, to avoid issues when the spreadsheet is not updated according to the current date
- Added the 'fixed_income_test.py' file, in order to test the simulations related to the fixed income calculation
- Updated the economic indexers spreadsheets
- Small refactoring to old related code
</commit_message>
<xml_diff>
--- a/indexer_lib/data/Poupança nova mensal.xlsx
+++ b/indexer_lib/data/Poupança nova mensal.xlsx
@@ -423,9 +423,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -514,7 +512,9 @@
       <c r="L2" s="3">
         <v>0.44</v>
       </c>
-      <c r="M2" s="3"/>
+      <c r="M2" s="3">
+        <v>0.63</v>
+      </c>
       <c r="O2" t="s">
         <v>15</v>
       </c>

</xml_diff>